<commit_message>
updates with vertical fault
</commit_message>
<xml_diff>
--- a/data/data_seismic/Fault_data.xlsx
+++ b/data/data_seismic/Fault_data.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="476" documentId="8_{E765D84F-7BB7-44A0-97F0-5D6C14C8947E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D237D071-C3FD-43E0-916D-450508150B1D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="5" xr2:uid="{BD47825D-16C2-4B40-91F8-9279CB178C7A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{BD47825D-16C2-4B40-91F8-9279CB178C7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fault_1" sheetId="1" r:id="rId1"/>
@@ -1738,17 +1738,17 @@
       <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>367902.40999999898</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>-20.151747034211887</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>368275.51</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>-20.151747034211887</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>368648.80999999901</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>-20.151747034211887</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>369022.51</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>-20.151747034211887</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>369395.609999999</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>-20.151747034211887</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>369863.01</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>-20.151747034211887</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>370329.51</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>-20.151747034211887</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>370797.01</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>-20.151747034211887</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>371264.609999999</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>-20.151747034211887</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>368225.609999999</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>368645.30999999901</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>368971.90999999898</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>369186.30999999901</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>369391.30999999901</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>369624.40999999898</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>369857.71</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>370091.01</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>370277.609999999</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>370557.21</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>370929.51</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>371395.51</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>-5.9315269249197637</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>371610.30999999901</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>371845.109999999</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>371938.90999999898</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>371985.90999999898</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>372126.609999999</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>372314.40999999898</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>372596.40999999898</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>373066.51</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>372128.01</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>372490.609999999</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>372807.40999999898</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>373033.51</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>373304.90999999898</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>373576.609999999</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>373848.30999999901</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>374120.01</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>356730.06271776999</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>356821.229965156</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>356912.397212543</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>357003.56445993</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>357094.731707317</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>357185.89895470301</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>357295.29965156701</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>357413.81707316998</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>357596.15156794398</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>357915.23693379702</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>358279.90592334402</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>358735.74216027802</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>-33.690067525979785</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>374000</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>373000</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>374000</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>375000</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>374000</v>
       </c>
@@ -3027,14 +3027,14 @@
       <selection activeCell="D2" sqref="D2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>371610.609999999</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>371713.40999999898</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>371825.609999999</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>371937.71</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>372049.90999999898</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>372162.01</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>372264.71</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>371582.30999999901</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>371442.21</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>371302.21</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>371208.90999999898</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>371162.30999999901</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>371115.71</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>371069.109999999</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>371022.609999999</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>370976.01</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>8.5314089990119957</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>370929.51</v>
       </c>
@@ -3462,15 +3462,15 @@
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>374018.21</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>18.141933233947686</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>374492.30999999901</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>18.141933233947686</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>374979.30999999901</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>18.141933233947686</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>375421.21</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>18.141933233947686</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>375764.609999999</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>18.141933233947686</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>376009.71</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>18.141933233947686</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>376204.609999999</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>18.141933233947686</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>373345.34615384601</v>
       </c>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>373970.73076922999</v>
       </c>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>374471.03846153797</v>
       </c>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>374908.80769230699</v>
       </c>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>375221.5</v>
       </c>
@@ -3774,7 +3774,7 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>375534.19230769202</v>
       </c>
@@ -3798,7 +3798,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>375846.88461538398</v>
       </c>
@@ -3831,19 +3831,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F4AAE1-3020-45D4-A8E8-7DE3FE904ED5}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>377812.109999999</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>378092.21</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>378465.40999999898</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>378885.01</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>379211.109999999</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>379489.609999999</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>379673.21</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>379855.01</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>380041.609999999</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>376315.92307692301</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>376941.30769230699</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>377660.5</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>378348.42307692301</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>379130.153846153</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>379911.88461538398</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>13.640502536954809</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>380693.61538461503</v>
       </c>
@@ -4248,14 +4248,14 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>400705.92307692301</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>399767.84615384601</v>
       </c>
@@ -4325,7 +4325,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>409317</v>
       </c>
@@ -4357,18 +4357,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D339F6BC-4E90-4E9D-A8EF-D6DADAFB3F24}">
   <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+    <sheetView topLeftCell="A110" workbookViewId="0">
       <selection activeCell="I129" sqref="I129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>365091.01</v>
       </c>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>366030.609999999</v>
       </c>
@@ -4403,7 +4403,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>366966.40999999898</v>
       </c>
@@ -4415,7 +4415,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>367902.40999999898</v>
       </c>
@@ -4427,7 +4427,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>369769.40999999898</v>
       </c>
@@ -4440,7 +4440,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>370703.51</v>
       </c>
@@ -4452,7 +4452,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>371638.609999999</v>
       </c>
@@ -4464,7 +4464,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>372572.30999999901</v>
       </c>
@@ -4476,7 +4476,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>373504.609999999</v>
       </c>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>373971.40999999898</v>
       </c>
@@ -4501,7 +4501,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>374444.30999999901</v>
       </c>
@@ -4513,7 +4513,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>375421.21</v>
       </c>
@@ -4525,7 +4525,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>376402.71</v>
       </c>
@@ -4537,7 +4537,7 @@
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>377345.21</v>
       </c>
@@ -4549,7 +4549,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>378279.01</v>
       </c>
@@ -4561,7 +4561,7 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>379211.109999999</v>
       </c>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>380135.01</v>
       </c>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>381067.609999999</v>
       </c>
@@ -4597,7 +4597,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>366734.51</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>-3041.3452189282002</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>367200.21</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>-3041.3452189282002</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>367666.21</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>-3041.3452189282002</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>368132.30999999901</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>-3079.5569928668401</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>368598.71</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>-3117.9649703313498</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>371022.609999999</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>-1324.7014327480699</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>371395.51</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>-1324.7014327480699</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>371862.40999999898</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>-1324.7014327480699</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>372799.01</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>-1380.91601746219</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>373761.80999999901</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>-1554.2686562251199</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>374729.01</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>-1673.7611525841901</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>370904.90999999898</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>-2183.1237021574402</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>371281.01</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>-2250.3256843195099</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>372220.51</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>-1296.88844567979</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>372690.40999999898</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>-1269.27166213736</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>373160.40999999898</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>-1225.4929118032701</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>373629.71</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>-1214.6267056300801</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>374098.40999999898</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>-1214.6267056300801</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>374560.90999999898</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>-1241.8510821207999</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>375018.40999999898</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>-1554.2686562251199</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>375474.51</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>-1583.84747502611</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>375928.90999999898</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>-1613.6224973529499</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>376381.21</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>-1643.5937232056399</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>376833.609999999</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>-1673.7611525841901</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>377287.90999999898</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>-1734.6846219188701</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>377742.21</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>-1808.82873973699</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>371057.30999999901</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>-2116.7065340988001</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>371494.90999999898</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>-2116.7065340988001</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>371946.609999999</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>-1986.2266402917901</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>372400.01</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>-1954.0971756546801</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>374210.609999999</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>-1241.8510821207999</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>374663.609999999</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>-1269.27166213736</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>375120.21</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>-1324.7014327480699</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>375680.90999999898</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>-1613.6224973529499</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>376058.01</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>-1643.5937232056399</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>376530.40999999898</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>-1673.7611525841901</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>377010.109999999</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>-1673.7611525841901</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>377481.109999999</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>-1704.1247854886001</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>377951.90999999898</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>-1734.6846219188701</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>378422.90999999898</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>-1796.39290535696</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>378901.51</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>-1890.4268569580299</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>379369.21</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>-1973.35131001385</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>377384.80999999901</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>-2018.5523084547599</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>377256.90999999898</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>-2018.5523084547599</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>377121.90999999898</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>-1986.2266402917901</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>376988.01</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>-1954.0971756546801</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>376852.21</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>-1922.1639145434301</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>376715.90999999898</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>-1922.1639145434301</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>376592.30999999901</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>-1922.1639145434301</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>376447.609999999</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>-1922.1639145434301</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>376248.40999999898</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>-1922.1639145434301</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>376040.21</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>-1922.1639145434301</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>375831.90999999898</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>-1890.4268569580299</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>375580.609999999</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>-1890.4268569580299</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>375414.01</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>-1890.4268569580299</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>375205.30999999901</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>-1890.4268569580299</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>376796.51</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>-1613.6224973529499</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>376471.90999999898</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>-1613.6224973529499</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>376150.40999999898</v>
       </c>
@@ -5246,7 +5246,7 @@
         <v>-1613.6224973529499</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>375823.21</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>-1613.6224973529499</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>375500.40999999898</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>-1613.6224973529499</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>374537.90999999898</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>-1269.27166213736</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>374241.30999999901</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>-1241.8510821207999</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>373980.30999999901</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>-1214.6267056300801</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>373727.40999999898</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>-1214.6267056300801</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>373464.71</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>-1187.5985326652301</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>373217.40999999898</v>
       </c>
@@ -5334,7 +5334,7 @@
         <v>-1187.5985326652301</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>372725.40999999898</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>-1214.6267056300801</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>372476.21</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>-1241.8510821207999</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>372232.51</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>-1269.27166213736</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>371978.21</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>-1296.88844567979</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>371722.90999999898</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>-1324.7014327480699</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>371452.609999999</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>-1296.88844567979</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>369900.30999999901</v>
       </c>
@@ -5411,7 +5411,7 @@
         <v>-3041.3452189282002</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>369660.51</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>-3041.3452189282002</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>369188.609999999</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>-2816.1948493392802</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>368949.71</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>-2816.1948493392802</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>368710.21</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>-2779.3565000816302</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>368468.21</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>-2779.3565000816302</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>360293.73839662399</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>-5681.3318960121996</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>361119.47679324797</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>-5192.2832350341996</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>361945.21518987301</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>-4815.1709601134298</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>362770.95358649699</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>-4361.43893378951</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>363596.69198312197</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>-3676.2780250492801</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>364339.856540084</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>-3512.83593889847</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>364670.15189873398</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>-3635.1231982228001</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>364835.299578059</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>-3553.4021551473902</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>369124</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>-2250.3256843195099</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>370687.46153846098</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>-2216.62659147555</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>372250.92307692301</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>-2352.6001840065201</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>373814.38461538398</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>-2562.4466785786699</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>375377.84615384601</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>-2491.7130329511901</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>376941.30769230699</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>-2706.2684121438801</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>378817.46153846098</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>-2598.1078066811901</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>380068.23076922999</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>-2742.71435434983</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>381631.69230769202</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>-2890.4601584321599</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>383195.153846153</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>-3003.3296485154001</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>384758.61538461503</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>-3041.3452189282002</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>386947.46153846098</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>-3312.9479105417099</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>387416.5</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>-3234.36612387999</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>387885.53846153797</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>-3234.36612387999</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>389449</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>-3352.5331091613498</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>391012.46153846098</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>-3594.1645749221598</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>392575.92307692301</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>-4185.4398219839104</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>394139.38461538398</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>-4185.4398219839104</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>395702.84615384601</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>-4540.5773020088</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>397266.30769230699</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>-4908.2718076884803</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>398829.76923076902</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>-5049.3946054949902</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>373292</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>-3273.5589154479198</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>374308.43564356398</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>-3273.5589154479198</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>375324.87128712801</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>-3273.5589154479198</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>376341.30693069298</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>-3195.36953583792</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>377357.74257425702</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>-3156.5691513217098</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>378374.178217821</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>-3117.9649703313498</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>379390.61386138602</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>-3079.5569928668401</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>380407.04950495</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>-3003.3296485154001</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>381423.48514851398</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>-2927.8871182673902</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>382439.92079207901</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>-2890.4601584321599</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>383456.35643564299</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>-2853.2294021227899</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>384472.79207920702</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>-2816.1948493392802</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>385489.22772277199</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>-2816.1948493392802</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>386505.66336633603</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>-2779.3565000816302</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>386708.95049504901</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>-3676.2780250492801</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>387522.0990099</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>-3676.2780250492801</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>388538.53465346497</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>-3594.1645749221598</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>389554.97029702901</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>-3594.1645749221598</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>390571.40594059398</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>-3635.1231982228001</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>391587.84158415801</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>-3676.2780250492801</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>392604.27722772199</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>-3759.1762892798301</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>393620.71287128702</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>-3842.8593676137998</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>394637.148514851</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>-3927.32726005119</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>395653.58415841497</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>-4012.5799665919999</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>396670.01980198</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>-4185.4398219839104</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>397686.45544554398</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>-4273.0469708350001</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>398702.89108910802</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>-4450.6157108474399</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>399719.32673267298</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>-4540.5773020088</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>400735.76237623702</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>-4631.3237072735901</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>401752.198019801</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>-4722.8549266418004</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>402768.63366336602</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>-4908.2718076884803</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>403785.06930693</v>
       </c>

</xml_diff>